<commit_message>
Tkinter Email list + attaching files
</commit_message>
<xml_diff>
--- a/Book23.xlsx
+++ b/Book23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s_pasiukevich/PycharmProjects/pythonProject6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E6E293-E3D9-3643-94C1-D8D4FAAE43BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC8BDF9-4A62-DD4D-A903-C4D42A862E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{B854FBF5-E01D-414A-8385-543F6769E8AD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>+375295006019</t>
   </si>
@@ -107,6 +107,24 @@
   </si>
   <si>
     <t>a_kasach@lesta.group</t>
+  </si>
+  <si>
+    <t>d_kirol@lesta.group</t>
+  </si>
+  <si>
+    <t>d_kireev@lesta.group</t>
+  </si>
+  <si>
+    <t>d_kinov@lesta.group</t>
+  </si>
+  <si>
+    <t>d_karin@lesta.group</t>
+  </si>
+  <si>
+    <t>a_dyshina@lesta.group</t>
+  </si>
+  <si>
+    <t>e_semenova@lesta.group</t>
   </si>
 </sst>
 </file>
@@ -477,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5353B35E-7418-B747-9CF7-4B0932CBA9BD}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,6 +605,36 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -606,6 +654,12 @@
     <hyperlink ref="A13" r:id="rId12" xr:uid="{93757910-3230-C341-8048-D1BE2F5C72A0}"/>
     <hyperlink ref="A14" r:id="rId13" xr:uid="{66F5B918-9D31-0941-92C7-E852DE1FC5E8}"/>
     <hyperlink ref="A15" r:id="rId14" xr:uid="{19F1C380-3F05-2143-82C0-12A685722147}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{8F478736-CBF1-2A42-AD3B-D42FDA884B2A}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{A91FCFD2-AE58-7846-A7E7-125772C763BF}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{0E3B797D-A3B9-A84C-AF1B-81FC86C8BC9C}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{E2BE3635-3945-014E-8997-136A3743D591}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{7FE10F74-97C5-BB45-B98F-08B99C206941}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{3D2C535E-317C-334F-9102-74EEA1BE8A73}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>